<commit_message>
Update GUI and data files: fix CSV parsing and file references
</commit_message>
<xml_diff>
--- a/sintesi ipotesi.xlsx
+++ b/sintesi ipotesi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentiuniparthenope-my.sharepoint.com/personal/pietro_maietta001_studenti_uniparthenope_it/Documents/tesi/Tesi Magistrale/Tesi-Magistrale_backup0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{53B4FCD8-DCCC-42C2-8284-60FDE9002A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{53B4FCD8-DCCC-42C2-8284-60FDE9002A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC623852-E5FB-4171-BBDE-B18DB13309CC}"/>
   <bookViews>
-    <workbookView xWindow="3696" yWindow="1860" windowWidth="17280" windowHeight="8880" xr2:uid="{EED7F668-7CF6-47D9-9053-7172807BEABC}"/>
+    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8880" xr2:uid="{EED7F668-7CF6-47D9-9053-7172807BEABC}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>Ipotesi</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Segno atteso</t>
   </si>
   <si>
-    <t>Segno stimato</t>
-  </si>
-  <si>
     <t>p-value</t>
   </si>
   <si>
@@ -62,57 +59,34 @@
     <t>H1</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">L’ISP presenta una </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>correlazione positiva</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> e significativa con gli indicatori di equilibrio economico (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>ROE, ROS</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>), confermando la sua capacità di sintetizzare la redditività aziendale.</t>
-    </r>
-  </si>
-  <si>
     <t>+</t>
   </si>
   <si>
-    <t>&lt; 0.001</t>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>H3</t>
+  </si>
+  <si>
+    <t>≠</t>
+  </si>
+  <si>
+    <t>H4</t>
+  </si>
+  <si>
+    <t>Evidenza stimata</t>
+  </si>
+  <si>
+    <t>La performance economico-finanziaria (ISP) dipende significativamente dagli indicatori di redditività, solidità e liquidità.</t>
+  </si>
+  <si>
+    <t>+ / –</t>
+  </si>
+  <si>
+    <t>ROI, ROE, indici di liquidità positivi; indipendenza finanziaria e indebitamento eccessivo negativi</t>
+  </si>
+  <si>
+    <t>&lt; 0,001</t>
   </si>
   <si>
     <r>
@@ -120,204 +94,49 @@
     </r>
     <r>
       <rPr>
-        <i/>
-        <sz val="12"/>
+        <sz val="9"/>
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve"> </t>
+      <t xml:space="preserve"> Confermata</t>
     </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Confermata</t>
-    </r>
-  </si>
-  <si>
-    <t>ROE e ROS positivi e altamente significativi in tutti i modelli. L’ISP riflette correttamente la componente reddituale.</t>
-  </si>
-  <si>
-    <t>H2</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">L’ISP mostra una </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>correlazione negativa</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> con gli indicatori di indebitamento e coerente con gli indici di liquidità, riflettendo l’equilibrio patrimoniale-finanziario dell’impresa.</t>
-    </r>
-  </si>
-  <si>
-    <t>–</t>
-  </si>
-  <si>
-    <t>– / ±</t>
-  </si>
-  <si>
-    <r>
-      <t>⚖️</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Parzialmente confermata</t>
-    </r>
-  </si>
-  <si>
-    <t>Debiti bancari e oneri finanziari negativi; coverage e leverage positivi, segno di leva sostenibile.</t>
-  </si>
-  <si>
-    <t>H3</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">L’impatto dei principali indicatori economico-finanziari sull’ISP differisce tra </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>macro-aree geografiche</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> (Nord, Centro, Sud).</t>
-    </r>
-  </si>
-  <si>
-    <t>≠</t>
-  </si>
-  <si>
-    <t>&lt; 0.01</t>
-  </si>
-  <si>
-    <t>Eterogeneità territoriale: cluster di performance più elevata nel Nord-Ovest.</t>
-  </si>
-  <si>
-    <t>H4</t>
-  </si>
-  <si>
-    <r>
-      <t>Le misure di autocorrelazione locale (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>LISA</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Getis-Ord Gi*</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> ) mostrano </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>cluster significativi</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> di imprese con performance simili.</t>
-    </r>
-  </si>
-  <si>
-    <t>Evidenza di hotspot ad alta performance nel Nord e lungo la dorsale tirrenica.</t>
+  </si>
+  <si>
+    <t>L’ISP sintetizza coerentemente le componenti economiche e finanziarie; la redditività emerge come principale driver della performance.</t>
+  </si>
+  <si>
+    <t>Esistono differenze strutturali tra le classi dimensionali (micro, piccole, medie, grandi) nella determinazione della performance.</t>
+  </si>
+  <si>
+    <t>Coefficienti e R² variabili per dimensione; ROI/ROE forti per tutte, IV più penalizzante per le micro</t>
+  </si>
+  <si>
+    <t>&lt; 0,01</t>
+  </si>
+  <si>
+    <t>Differenze significative nei driver di performance: effetto scala e struttura finanziaria più rilevanti per le imprese maggiori.</t>
+  </si>
+  <si>
+    <t>Le performance d’impresa mostrano autocorrelazione spaziale, con cluster di alta o bassa performance.</t>
+  </si>
+  <si>
+    <t>Cluster HH e LL significativi (LISA, Gi*); autocorrelazione positiva ma contenuta</t>
+  </si>
+  <si>
+    <t>Evidenza di concentrazioni territoriali coerenti con la geografia economica italiana (Nord vs Sud).</t>
+  </si>
+  <si>
+    <t>Le relazioni spaziali influenzano la performance attraverso effetti di spillover e interdipendenza locale.</t>
+  </si>
+  <si>
+    <t>+ / ±</t>
+  </si>
+  <si>
+    <t>ρ significativo nei modelli SAR/SDM; spillover positivi di solidità e liquidità</t>
+  </si>
+  <si>
+    <t>Effetti diretti e indiretti rilevanti nei contesti ad alta densità produttiva; interdipendenza più debole nel Mezzogiorno.</t>
   </si>
 </sst>
 </file>
@@ -334,22 +153,19 @@
     </font>
     <font>
       <b/>
-      <i/>
-      <sz val="12"/>
+      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
     <font>
-      <i/>
-      <sz val="12"/>
+      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
     <font>
-      <i/>
-      <sz val="12"/>
+      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Segoe UI Emoji"/>
       <family val="2"/>
@@ -363,7 +179,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -386,20 +202,64 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+      <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -738,124 +598,133 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G5"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="3"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="65.400000000000006" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:7" ht="180.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="B2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:7" ht="156.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="144.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="D4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="144.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="B5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="F5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="315" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="316.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>26</v>
+      <c r="G5" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>